<commit_message>
Enhanced Pedestrian Motion over Large Grids
Pedestrians now flow into alternate paths, converge and move towards
goals in a more realistic manner.
Cells now give values in an unexponentiated manner.
Changed Pedestrian RequestMove a lot to accommodate this. Also made
Pedestrian methods more efficient.
Walls, roads and cells now color themselves much better.
</commit_message>
<xml_diff>
--- a/EvacMap.xlsx
+++ b/EvacMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="8">
   <si>
     <t>open</t>
   </si>
@@ -30,16 +30,19 @@
     <t>wall</t>
   </si>
   <si>
-    <t>exit</t>
-  </si>
-  <si>
     <t>wall-d</t>
   </si>
   <si>
-    <t>stoplight</t>
+    <t>crosswalk</t>
   </si>
   <si>
-    <t>crosswalk</t>
+    <t>stoplight 300 400</t>
+  </si>
+  <si>
+    <t>exit 50</t>
+  </si>
+  <si>
+    <t>exit 51</t>
   </si>
 </sst>
 </file>
@@ -370,8 +373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -462,10 +465,10 @@
         <v>0</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>0</v>
@@ -1540,8 +1543,8 @@
       <c r="AU8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AV8" s="1" t="s">
-        <v>3</v>
+      <c r="AV8" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1686,8 +1689,8 @@
       <c r="AU9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AV9" s="1" t="s">
-        <v>3</v>
+      <c r="AV9" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1832,8 +1835,8 @@
       <c r="AU10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AV10" s="1" t="s">
-        <v>3</v>
+      <c r="AV10" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1883,7 +1886,7 @@
         <v>2</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>0</v>
@@ -1894,29 +1897,29 @@
       <c r="S11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB11" s="1" t="s">
         <v>0</v>
@@ -2040,29 +2043,29 @@
       <c r="S12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>0</v>
@@ -2186,29 +2189,29 @@
       <c r="S13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>0</v>
@@ -2332,29 +2335,29 @@
       <c r="S14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>0</v>
@@ -2478,29 +2481,29 @@
       <c r="S15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>0</v>
@@ -2624,29 +2627,29 @@
       <c r="S16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="T16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>0</v>
@@ -2759,7 +2762,7 @@
         <v>2</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Enhanced Pedestrian Motion and Stoplights
Stoplights now take in starting offset to allow for staggered lights
Pedestrians now don’t have a propagation delay in crowds
Cell drawing and Stoplight drawing better
</commit_message>
<xml_diff>
--- a/EvacMap.xlsx
+++ b/EvacMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="9">
   <si>
     <t>open</t>
   </si>
@@ -36,13 +36,16 @@
     <t>crosswalk</t>
   </si>
   <si>
-    <t>stoplight 300 400</t>
-  </si>
-  <si>
     <t>exit 50</t>
   </si>
   <si>
     <t>exit 51</t>
+  </si>
+  <si>
+    <t>stoplight 300 400 350</t>
+  </si>
+  <si>
+    <t>stoplight 400 300 0</t>
   </si>
 </sst>
 </file>
@@ -373,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -465,10 +468,10 @@
         <v>0</v>
       </c>
       <c r="AC1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>0</v>
@@ -1898,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>4</v>
@@ -2044,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>4</v>
@@ -2190,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>4</v>
@@ -2336,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>4</v>
@@ -2482,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>4</v>
@@ -2628,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>4</v>

</xml_diff>